<commit_message>
Added 20k offset figures
</commit_message>
<xml_diff>
--- a/data/fig2in.xlsx
+++ b/data/fig2in.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/covid_cea/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Howard\Documents\Bristol\Covid-19\Cost-effectiveness of lockdowns\covid_cea\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D10719B-CA5A-2B4D-AFB8-0CED8BAB78FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3801285E-4AAB-4CE1-A40B-4D55E93D8654}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{5997DEA7-33B8-4C4B-BAE2-CF09A3FC7B11}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13155" xr2:uid="{5997DEA7-33B8-4C4B-BAE2-CF09A3FC7B11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>Country</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>MeanAge</t>
+  </si>
+  <si>
+    <t>Recoup20k</t>
   </si>
 </sst>
 </file>
@@ -496,15 +499,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C46B683-D0FF-6348-BD79-699FC6CA61E5}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,13 +530,16 @@
         <v>11</v>
       </c>
       <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -556,13 +562,16 @@
         <v>61.2</v>
       </c>
       <c r="H2">
+        <v>46.1</v>
+      </c>
+      <c r="I2">
         <v>5.7542595054321986</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -585,13 +594,16 @@
         <v>39.700000000000003</v>
       </c>
       <c r="H3">
+        <v>29.8</v>
+      </c>
+      <c r="I3">
         <v>3.9622449602689445</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -614,13 +626,16 @@
         <v>67.8</v>
       </c>
       <c r="H4">
+        <v>51</v>
+      </c>
+      <c r="I4">
         <v>6.0464305063217187</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -643,13 +658,16 @@
         <v>95</v>
       </c>
       <c r="H5">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="I5">
         <v>6.0173296180811073</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -672,13 +690,16 @@
         <v>87.9</v>
       </c>
       <c r="H6">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="I6">
         <v>5.6283889690439866</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -701,13 +722,16 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="H7">
+        <v>7.17</v>
+      </c>
+      <c r="I7">
         <v>1.0455423114875257</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -730,13 +754,16 @@
         <v>17.899999999999999</v>
       </c>
       <c r="H8">
+        <v>13.6</v>
+      </c>
+      <c r="I8">
         <v>1.8071929201075876</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -759,13 +786,16 @@
         <v>15.8</v>
       </c>
       <c r="H9">
+        <v>12.5</v>
+      </c>
+      <c r="I9">
         <v>1.5669747391252111</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -788,13 +818,16 @@
         <v>12.4</v>
       </c>
       <c r="H10">
+        <v>9.68</v>
+      </c>
+      <c r="I10">
         <v>0.69793768184117033</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -817,13 +850,16 @@
         <v>30.6</v>
       </c>
       <c r="H11">
+        <v>23.6</v>
+      </c>
+      <c r="I11">
         <v>2.0507594425562732</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -846,13 +882,16 @@
         <v>70.7</v>
       </c>
       <c r="H12">
+        <v>53.2</v>
+      </c>
+      <c r="I12">
         <v>6.6689972408925948</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -875,13 +914,16 @@
         <v>48.1</v>
       </c>
       <c r="H13">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="I13">
         <v>4.8206904941905888</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -904,13 +946,16 @@
         <v>81.400000000000006</v>
       </c>
       <c r="H14">
+        <v>61.2</v>
+      </c>
+      <c r="I14">
         <v>7.2675312745118639</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -933,13 +978,16 @@
         <v>114.5</v>
       </c>
       <c r="H15">
+        <v>85.7</v>
+      </c>
+      <c r="I15">
         <v>7.3471989516015759</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -962,9 +1010,12 @@
         <v>105.6</v>
       </c>
       <c r="H16">
+        <v>79.5</v>
+      </c>
+      <c r="I16">
         <v>6.7677110005356163</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>41</v>
       </c>
     </row>

</xml_diff>